<commit_message>
db id to db name
</commit_message>
<xml_diff>
--- a/Backend/uploads/test2407new 1_2_3_4_5.xlsx
+++ b/Backend/uploads/test2407new 1_2_3_4_5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Raghav/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8396C6F4-D043-8D47-A5AE-92EF5B5AA5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59947D44-1097-724D-AA11-D31E68780FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{43E4022F-9CEB-4BCA-804E-CA3014EB1CE3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>Sl.No</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>verify the status</t>
+  </si>
+  <si>
+    <t>Snowflake</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -672,11 +675,11 @@
         <v>7</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
+      <c r="E2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -695,11 +698,11 @@
         <v>8</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
@@ -718,11 +721,11 @@
         <v>9</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
+      <c r="E4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
@@ -741,11 +744,11 @@
         <v>10</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
+      <c r="E5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>6</v>
@@ -764,11 +767,11 @@
         <v>11</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>6</v>
@@ -787,11 +790,11 @@
         <v>12</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>6</v>
@@ -810,11 +813,11 @@
         <v>13</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
+      <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>6</v>
@@ -833,11 +836,11 @@
         <v>14</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
+      <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>6</v>
@@ -856,11 +859,11 @@
         <v>15</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
+      <c r="E10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>6</v>
@@ -879,11 +882,11 @@
         <v>16</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>6</v>
@@ -902,11 +905,11 @@
         <v>28</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="7">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7">
-        <v>1</v>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>6</v>
@@ -923,11 +926,11 @@
         <v>31</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="7">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>1</v>
+      <c r="E13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>6</v>
@@ -944,11 +947,11 @@
         <v>33</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="E14" s="7">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7">
-        <v>1</v>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>6</v>
@@ -965,11 +968,11 @@
         <v>34</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7">
-        <v>1</v>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>6</v>
@@ -986,11 +989,11 @@
         <v>36</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="7">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7">
-        <v>1</v>
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>6</v>
@@ -1007,11 +1010,11 @@
         <v>39</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
+      <c r="E17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>6</v>
@@ -1030,11 +1033,11 @@
       <c r="D18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="5">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1</v>
+      <c r="E18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>6</v>
@@ -1245,6 +1248,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e11ba969-f758-4175-89cb-599b9be7130c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9CA0C431ACA584986A8DCF23B6B68D1" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eff462f0df5707225c4068d54027ad9d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e11ba969-f758-4175-89cb-599b9be7130c" xmlns:ns4="159d2a1b-2e76-4ffd-ac63-e9ef7d025ee8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6dc1120a2e184c0a420282cb888421c2" ns3:_="" ns4:_="">
     <xsd:import namespace="e11ba969-f758-4175-89cb-599b9be7130c"/>
@@ -1465,14 +1476,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e11ba969-f758-4175-89cb-599b9be7130c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1483,6 +1486,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8AC271D-DADF-4259-90E5-808448D69A83}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="159d2a1b-2e76-4ffd-ac63-e9ef7d025ee8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e11ba969-f758-4175-89cb-599b9be7130c"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49239FC-DB5B-40CE-97F3-9FDAF2046A7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1501,23 +1521,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8AC271D-DADF-4259-90E5-808448D69A83}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="159d2a1b-2e76-4ffd-ac63-e9ef7d025ee8"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e11ba969-f758-4175-89cb-599b9be7130c"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50BB7106-C26C-430C-9618-D3F20AE89230}">
   <ds:schemaRefs>

</xml_diff>